<commit_message>
Intermediate code commit and updated the task sheet
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>S.No.</t>
   </si>
@@ -118,13 +118,37 @@
   </si>
   <si>
     <t>HTML Wireframes creation (Login, Account, Dashboard, Devices Scanner page etc)</t>
+  </si>
+  <si>
+    <t>Save Password</t>
+  </si>
+  <si>
+    <t>Login --&gt; Texboxes width increase</t>
+  </si>
+  <si>
+    <t>Texboxes content place holder</t>
+  </si>
+  <si>
+    <t>Form authentication. Redirect to login in case other url hit without login</t>
+  </si>
+  <si>
+    <t>Toastr for message</t>
+  </si>
+  <si>
+    <t>After login failed, no message shown to user.</t>
+  </si>
+  <si>
+    <t>Add User/ Manage Users</t>
+  </si>
+  <si>
+    <t>Left Side Menu, Role based.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +197,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -251,6 +280,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -285,6 +315,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,12 +491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="49.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -474,7 +507,7 @@
     <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -514,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -534,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -550,7 +583,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -566,7 +599,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -584,7 +617,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -601,7 +634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -613,7 +646,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -630,7 +663,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -647,7 +680,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -664,7 +697,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -681,7 +714,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -698,7 +731,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -715,7 +748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -732,7 +765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -747,469 +780,525 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -1222,24 +1311,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Other master pages added & Login layout rectified.
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$33</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="60">
   <si>
     <t>S.No.</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>Reporting</t>
+  </si>
+  <si>
+    <t>Facebook, Twitter, Integration</t>
+  </si>
+  <si>
+    <t>Vipin</t>
+  </si>
+  <si>
+    <t>Dependency Injection</t>
+  </si>
+  <si>
+    <t>Testing remaining</t>
   </si>
 </sst>
 </file>
@@ -537,7 +549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -878,10 +892,10 @@
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>46</v>
@@ -896,10 +910,10 @@
         <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>46</v>
@@ -1157,112 +1171,135 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5">
+    <row r="33" spans="1:7">
+      <c r="A33" s="2">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30">
+      <c r="A34" s="2">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:7">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:7">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:7">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:7">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:7">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:7">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:7">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:7">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:7">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:7">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:7">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:7">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:7">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1585,7 +1622,7 @@
       <c r="E93" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G25">
+  <autoFilter ref="A1:G33">
     <filterColumn colId="4"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1) toastr message implemented 2) Seed method rectified.
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$35</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
   <si>
     <t>S.No.</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Testing remaining</t>
+  </si>
+  <si>
+    <t>In case of any error, login page still show invalid user message</t>
   </si>
 </sst>
 </file>
@@ -549,9 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -946,10 +947,10 @@
         <v>34</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>47</v>
@@ -964,10 +965,10 @@
         <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>46</v>
@@ -1208,12 +1209,22 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+    <row r="35" spans="1:7" ht="30">
+      <c r="A35" s="2">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2"/>
@@ -1622,7 +1633,7 @@
       <c r="E93" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G33">
+  <autoFilter ref="A1:G35">
     <filterColumn colId="4"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1) Save Password work implemented. 2) Form Authentication redirect work done.
</commit_message>
<xml_diff>
--- a/Docs/Tasks.xlsx
+++ b/Docs/Tasks.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="65">
   <si>
     <t>S.No.</t>
   </si>
@@ -198,10 +198,22 @@
     <t>Dependency Injection</t>
   </si>
   <si>
-    <t>Testing remaining</t>
-  </si>
-  <si>
     <t>In case of any error, login page still show invalid user message</t>
+  </si>
+  <si>
+    <t>Login background image change</t>
+  </si>
+  <si>
+    <t>Sign Out</t>
+  </si>
+  <si>
+    <t>Put logged in user detail in session</t>
+  </si>
+  <si>
+    <t>Shambhoo/Vipin</t>
+  </si>
+  <si>
+    <t>Need to decide with Suraj</t>
   </si>
 </sst>
 </file>
@@ -724,7 +736,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -875,10 +887,10 @@
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>46</v>
@@ -932,7 +944,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>46</v>
@@ -1001,7 +1013,7 @@
         <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
@@ -1188,6 +1200,9 @@
       <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30">
       <c r="A34" s="2">
@@ -1200,21 +1215,19 @@
         <v>19</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="30">
       <c r="A35" s="2">
         <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>13</v>
@@ -1227,25 +1240,55 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2"/>
@@ -1633,7 +1676,8 @@
       <c r="E93" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G35">
+  <autoFilter ref="A1:G38">
+    <filterColumn colId="2"/>
     <filterColumn colId="4"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>